<commit_message>
Ordered according to excel sheet
</commit_message>
<xml_diff>
--- a/Order for WSN dec 2018.xlsx
+++ b/Order for WSN dec 2018.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="210" windowWidth="14355" windowHeight="7935"/>
+    <workbookView xWindow="-15" yWindow="5250" windowWidth="28830" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="116">
   <si>
     <t>Finse</t>
   </si>
@@ -362,6 +362,9 @@
   <si>
     <t>https://www.digikey.no/product-detail/en/hirose-electric-co-ltd/H4BBG-10102-Y6/H4BBG-10102-Y6-ND/425615</t>
   </si>
+  <si>
+    <t>https://www.digikey.no/product-detail/en/keystone-electronics/4688/36-4688-ND/4499297</t>
+  </si>
 </sst>
 </file>
 
@@ -481,27 +484,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -842,9 +825,9 @@
   <dimension ref="A1:AD1040"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="825" topLeftCell="A59" activePane="bottomLeft"/>
-      <selection sqref="A1:A73"/>
-      <selection pane="bottomLeft" sqref="A1:A77"/>
+      <pane ySplit="825" activePane="bottomLeft"/>
+      <selection sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="63.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,14 +927,16 @@
         <v>2</v>
       </c>
       <c r="K2" s="6">
-        <f t="shared" ref="K2:K16" si="0">SUM(E2:J2)</f>
+        <f>SUM(E2:J2)</f>
         <v>34</v>
       </c>
       <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
+      <c r="M2" s="6">
+        <v>34</v>
+      </c>
       <c r="N2" s="3">
         <f>K2-L2-M2</f>
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="O2" s="13"/>
       <c r="P2" s="5"/>
@@ -999,13 +984,13 @@
         <v>0</v>
       </c>
       <c r="K3" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(E3:J3)</f>
         <v>0</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3">
-        <f t="shared" ref="N3:N70" si="1">K3-L3-M3</f>
+        <f>K3-L3-M3</f>
         <v>0</v>
       </c>
       <c r="O3" s="11" t="s">
@@ -1053,7 +1038,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(E4:J4)</f>
         <v>0</v>
       </c>
       <c r="L4" s="3"/>
@@ -1092,14 +1077,16 @@
         <v>0</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(E5:J5)</f>
         <v>10</v>
       </c>
-      <c r="L5" s="3"/>
+      <c r="L5" s="3">
+        <v>20</v>
+      </c>
       <c r="M5" s="3"/>
       <c r="N5" s="3">
         <f>K5-L5-M5</f>
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="O5" s="11" t="s">
         <v>65</v>
@@ -1146,14 +1133,16 @@
         <v>0</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(E6:J6)</f>
         <v>10</v>
       </c>
-      <c r="L6" s="3"/>
+      <c r="L6" s="3">
+        <v>15</v>
+      </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f>K6-L6-M6</f>
+        <v>-5</v>
       </c>
       <c r="O6" s="11" t="s">
         <v>67</v>
@@ -1186,35 +1175,36 @@
         <v>4</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" ref="E7:E16" si="2">E$2*$D7</f>
+        <f>E$2*$D7</f>
         <v>40</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" ref="F7:J20" si="3">F$2*$D7</f>
+        <f>F$2*$D7</f>
         <v>40</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" si="3"/>
+        <f>G$2*$D7</f>
         <v>24</v>
       </c>
       <c r="H7" s="3">
-        <f t="shared" si="3"/>
+        <f>H$2*$D7</f>
         <v>8</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3">
-        <f t="shared" si="3"/>
+        <f>J$2*$D7</f>
         <v>8</v>
       </c>
       <c r="K7" s="3">
-        <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="L7" s="3"/>
+      <c r="L7" s="3">
+        <v>150</v>
+      </c>
       <c r="M7" s="3"/>
       <c r="N7" s="3">
-        <f t="shared" si="1"/>
-        <v>120</v>
+        <f>K7-L7-M7</f>
+        <v>-30</v>
       </c>
       <c r="O7" s="11" t="s">
         <v>66</v>
@@ -1247,35 +1237,37 @@
         <v>4</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" si="2"/>
+        <f>E$2*$D8</f>
         <v>40</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="3"/>
+        <f>F$2*$D8</f>
         <v>40</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" si="3"/>
+        <f>G$2*$D8</f>
         <v>24</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" si="3"/>
+        <f>H$2*$D8</f>
         <v>8</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3">
-        <f t="shared" si="3"/>
+        <f>J$2*$D8</f>
         <v>8</v>
       </c>
       <c r="K8" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(E8:J8)</f>
         <v>120</v>
       </c>
       <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
+      <c r="M8" s="3">
+        <v>120</v>
+      </c>
       <c r="N8" s="3">
-        <f t="shared" si="1"/>
-        <v>120</v>
+        <f>K8-L8-M8</f>
+        <v>0</v>
       </c>
       <c r="O8" s="11" t="s">
         <v>85</v>
@@ -1308,35 +1300,37 @@
         <v>4</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" si="2"/>
+        <f>E$2*$D9</f>
         <v>40</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="3"/>
+        <f>F$2*$D9</f>
         <v>40</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="3"/>
+        <f>G$2*$D9</f>
         <v>24</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" si="3"/>
+        <f>H$2*$D9</f>
         <v>8</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3">
-        <f t="shared" si="3"/>
+        <f>J$2*$D9</f>
         <v>8</v>
       </c>
       <c r="K9" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(E9:J9)</f>
         <v>120</v>
       </c>
       <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
+      <c r="M9" s="3">
+        <v>120</v>
+      </c>
       <c r="N9" s="3">
-        <f t="shared" si="1"/>
-        <v>120</v>
+        <f>K9-L9-M9</f>
+        <v>0</v>
       </c>
       <c r="O9" s="11" t="s">
         <v>85</v>
@@ -1369,28 +1363,28 @@
         <v>4</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" si="2"/>
+        <f>E$2*$D10</f>
         <v>40</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="3"/>
+        <f>F$2*$D10</f>
         <v>40</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" si="3"/>
+        <f>G$2*$D10</f>
         <v>24</v>
       </c>
       <c r="H10" s="3">
-        <f t="shared" si="3"/>
+        <f>H$2*$D10</f>
         <v>8</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3">
-        <f t="shared" si="3"/>
+        <f>J$2*$D10</f>
         <v>8</v>
       </c>
       <c r="K10" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(E10:J10)</f>
         <v>120</v>
       </c>
       <c r="L10" s="3">
@@ -1398,7 +1392,7 @@
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3">
-        <f t="shared" si="1"/>
+        <f>K10-L10-M10</f>
         <v>0</v>
       </c>
       <c r="O10" s="12" t="s">
@@ -1432,28 +1426,28 @@
         <v>2</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" si="2"/>
+        <f>E$2*$D11</f>
         <v>20</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" si="3"/>
+        <f>F$2*$D11</f>
         <v>20</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" si="3"/>
+        <f>G$2*$D11</f>
         <v>12</v>
       </c>
       <c r="H11" s="3">
-        <f t="shared" si="3"/>
+        <f>H$2*$D11</f>
         <v>4</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3">
-        <f t="shared" si="3"/>
+        <f>J$2*$D11</f>
         <v>4</v>
       </c>
       <c r="K11" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(E11:J11)</f>
         <v>60</v>
       </c>
       <c r="L11" s="3">
@@ -1461,7 +1455,7 @@
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3">
-        <f t="shared" si="1"/>
+        <f>K11-L11-M11</f>
         <v>0</v>
       </c>
       <c r="O11" s="12" t="s">
@@ -1495,28 +1489,28 @@
         <v>1</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" si="2"/>
+        <f>E$2*$D12</f>
         <v>10</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="3"/>
+        <f>F$2*$D12</f>
         <v>10</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" si="3"/>
+        <f>G$2*$D12</f>
         <v>6</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" si="3"/>
+        <f>H$2*$D12</f>
         <v>2</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3">
-        <f t="shared" si="3"/>
+        <f>J$2*$D12</f>
         <v>2</v>
       </c>
       <c r="K12" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(E12:J12)</f>
         <v>30</v>
       </c>
       <c r="L12" s="3">
@@ -1524,7 +1518,7 @@
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3">
-        <f t="shared" si="1"/>
+        <f>K12-L12-M12</f>
         <v>0</v>
       </c>
       <c r="O12" s="12" t="s">
@@ -1558,28 +1552,28 @@
         <v>1</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="2"/>
+        <f>E$2*$D13</f>
         <v>10</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="3"/>
+        <f>F$2*$D13</f>
         <v>10</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" si="3"/>
+        <f>G$2*$D13</f>
         <v>6</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" si="3"/>
+        <f>H$2*$D13</f>
         <v>2</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3">
-        <f t="shared" si="3"/>
+        <f>J$2*$D13</f>
         <v>2</v>
       </c>
       <c r="K13" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(E13:J13)</f>
         <v>30</v>
       </c>
       <c r="L13" s="3">
@@ -1587,7 +1581,7 @@
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3">
-        <f t="shared" si="1"/>
+        <f>K13-L13-M13</f>
         <v>0</v>
       </c>
       <c r="O13" s="12" t="s">
@@ -1621,28 +1615,28 @@
         <v>1</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="2"/>
+        <f>E$2*$D14</f>
         <v>10</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="3"/>
+        <f>F$2*$D14</f>
         <v>10</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" si="3"/>
+        <f>G$2*$D14</f>
         <v>6</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" si="3"/>
+        <f>H$2*$D14</f>
         <v>2</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3">
-        <f t="shared" si="3"/>
+        <f>J$2*$D14</f>
         <v>2</v>
       </c>
       <c r="K14" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(E14:J14)</f>
         <v>30</v>
       </c>
       <c r="L14" s="3"/>
@@ -1650,7 +1644,7 @@
         <v>30</v>
       </c>
       <c r="N14" s="3">
-        <f t="shared" si="1"/>
+        <f>K14-L14-M14</f>
         <v>0</v>
       </c>
       <c r="O14" s="11" t="s">
@@ -1684,28 +1678,28 @@
         <v>1</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="2"/>
+        <f>E$2*$D15</f>
         <v>10</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="3"/>
+        <f>F$2*$D15</f>
         <v>10</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" si="3"/>
+        <f>G$2*$D15</f>
         <v>6</v>
       </c>
       <c r="H15" s="3">
-        <f t="shared" si="3"/>
+        <f>H$2*$D15</f>
         <v>2</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3">
-        <f t="shared" si="3"/>
+        <f>J$2*$D15</f>
         <v>2</v>
       </c>
       <c r="K15" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(E15:J15)</f>
         <v>30</v>
       </c>
       <c r="L15" s="3"/>
@@ -1713,7 +1707,7 @@
         <v>30</v>
       </c>
       <c r="N15" s="3">
-        <f t="shared" si="1"/>
+        <f>K15-L15-M15</f>
         <v>0</v>
       </c>
       <c r="O15" s="11" t="s">
@@ -1747,37 +1741,39 @@
         <v>1</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="2"/>
+        <f>E$2*$D16</f>
         <v>10</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" si="3"/>
+        <f>F$2*$D16</f>
         <v>10</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" si="3"/>
+        <f>G$2*$D16</f>
         <v>6</v>
       </c>
       <c r="H16" s="3">
-        <f t="shared" si="3"/>
+        <f>H$2*$D16</f>
         <v>2</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3">
-        <f t="shared" si="3"/>
+        <f>J$2*$D16</f>
         <v>2</v>
       </c>
       <c r="K16" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(E16:J16)</f>
         <v>30</v>
       </c>
       <c r="L16" s="3">
         <v>10</v>
       </c>
-      <c r="M16" s="3"/>
+      <c r="M16" s="3">
+        <v>25</v>
+      </c>
       <c r="N16" s="3">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <f>K16-L16-M16</f>
+        <v>-5</v>
       </c>
       <c r="O16" s="12" t="s">
         <v>63</v>
@@ -1914,28 +1910,28 @@
         <v>1</v>
       </c>
       <c r="E20" s="3">
-        <f t="shared" ref="E20:E28" si="4">E$2*$D20</f>
+        <f>E$2*$D20</f>
         <v>10</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="3"/>
+        <f>F$2*$D20</f>
         <v>10</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" si="3"/>
+        <f>G$2*$D20</f>
         <v>6</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" si="3"/>
+        <f>H$2*$D20</f>
         <v>2</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3">
-        <f t="shared" si="3"/>
+        <f>J$2*$D20</f>
         <v>2</v>
       </c>
       <c r="K20" s="3">
-        <f t="shared" ref="K20:K29" si="5">SUM(E20:J20)</f>
+        <f>SUM(E20:J20)</f>
         <v>30</v>
       </c>
       <c r="L20" s="3">
@@ -1943,7 +1939,7 @@
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3">
-        <f t="shared" si="1"/>
+        <f>K20-L20-M20</f>
         <v>0</v>
       </c>
       <c r="O20" s="12" t="s">
@@ -1977,35 +1973,37 @@
         <v>2</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" si="4"/>
+        <f>E$2*$D21</f>
         <v>20</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" ref="F21:H28" si="6">F$2*$D21</f>
+        <f>F$2*$D21</f>
         <v>20</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="6"/>
+        <f>G$2*$D21</f>
         <v>12</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="6"/>
+        <f>H$2*$D21</f>
         <v>4</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3">
-        <f t="shared" ref="J21:J28" si="7">J$2*$D21</f>
+        <f>J$2*$D21</f>
         <v>4</v>
       </c>
       <c r="K21" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(E21:J21)</f>
         <v>60</v>
       </c>
       <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
+      <c r="M21" s="3">
+        <v>75</v>
+      </c>
       <c r="N21" s="3">
-        <f t="shared" si="1"/>
-        <v>60</v>
+        <f>K21-L21-M21</f>
+        <v>-15</v>
       </c>
       <c r="O21" s="11" t="s">
         <v>86</v>
@@ -2038,35 +2036,37 @@
         <v>2</v>
       </c>
       <c r="E22" s="3">
-        <f t="shared" si="4"/>
+        <f>E$2*$D22</f>
         <v>20</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="6"/>
+        <f>F$2*$D22</f>
         <v>20</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" si="6"/>
+        <f>G$2*$D22</f>
         <v>12</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" si="6"/>
+        <f>H$2*$D22</f>
         <v>4</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3">
-        <f t="shared" si="7"/>
+        <f>J$2*$D22</f>
         <v>4</v>
       </c>
       <c r="K22" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(E22:J22)</f>
         <v>60</v>
       </c>
       <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
+      <c r="M22" s="3">
+        <v>75</v>
+      </c>
       <c r="N22" s="3">
         <f>K22-L22-M22</f>
-        <v>60</v>
+        <v>-15</v>
       </c>
       <c r="O22" s="11" t="s">
         <v>89</v>
@@ -2099,28 +2099,28 @@
         <v>1</v>
       </c>
       <c r="E23" s="3">
-        <f t="shared" si="4"/>
+        <f>E$2*$D23</f>
         <v>10</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="6"/>
+        <f>F$2*$D23</f>
         <v>10</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" si="6"/>
+        <f>G$2*$D23</f>
         <v>6</v>
       </c>
       <c r="H23" s="3">
-        <f t="shared" si="6"/>
+        <f>H$2*$D23</f>
         <v>2</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3">
-        <f t="shared" si="7"/>
+        <f>J$2*$D23</f>
         <v>2</v>
       </c>
       <c r="K23" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(E23:J23)</f>
         <v>30</v>
       </c>
       <c r="L23" s="3">
@@ -2128,7 +2128,7 @@
       </c>
       <c r="M23" s="3"/>
       <c r="N23" s="3">
-        <f t="shared" si="1"/>
+        <f>K23-L23-M23</f>
         <v>2</v>
       </c>
       <c r="O23" s="12" t="s">
@@ -2162,34 +2162,34 @@
         <v>5</v>
       </c>
       <c r="E24" s="3">
-        <f t="shared" si="4"/>
+        <f>E$2*$D24</f>
         <v>50</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" si="6"/>
+        <f>F$2*$D24</f>
         <v>50</v>
       </c>
       <c r="G24" s="3">
-        <f t="shared" si="6"/>
+        <f>G$2*$D24</f>
         <v>30</v>
       </c>
       <c r="H24" s="3">
-        <f t="shared" si="6"/>
+        <f>H$2*$D24</f>
         <v>10</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3">
-        <f t="shared" si="7"/>
+        <f>J$2*$D24</f>
         <v>10</v>
       </c>
       <c r="K24" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(E24:J24)</f>
         <v>150</v>
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3">
-        <f t="shared" si="1"/>
+        <f>K24-L24-M24</f>
         <v>150</v>
       </c>
       <c r="O24" s="11" t="s">
@@ -2223,35 +2223,37 @@
         <v>6</v>
       </c>
       <c r="E25" s="3">
-        <f t="shared" si="4"/>
+        <f>E$2*$D25</f>
         <v>60</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" si="6"/>
+        <f>F$2*$D25</f>
         <v>60</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" si="6"/>
+        <f>G$2*$D25</f>
         <v>36</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" si="6"/>
+        <f>H$2*$D25</f>
         <v>12</v>
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3">
-        <f t="shared" si="7"/>
+        <f>J$2*$D25</f>
         <v>12</v>
       </c>
       <c r="K25" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(E25:J25)</f>
         <v>180</v>
       </c>
       <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
+      <c r="M25" s="3">
+        <v>200</v>
+      </c>
       <c r="N25" s="3">
-        <f t="shared" si="1"/>
-        <v>180</v>
+        <f>K25-L25-M25</f>
+        <v>-20</v>
       </c>
       <c r="O25" s="11" t="s">
         <v>93</v>
@@ -2284,35 +2286,36 @@
         <v>2</v>
       </c>
       <c r="E26" s="3">
-        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <f>F$2*$D26</f>
         <v>20</v>
       </c>
-      <c r="F26" s="3">
-        <f t="shared" si="6"/>
-        <v>20</v>
-      </c>
       <c r="G26" s="3">
-        <f t="shared" si="6"/>
+        <f>G$2*$D26</f>
         <v>12</v>
       </c>
       <c r="H26" s="3">
-        <f t="shared" si="6"/>
+        <f>H$2*$D26</f>
         <v>4</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3">
-        <f t="shared" si="7"/>
+        <f>J$2*$D26</f>
         <v>4</v>
       </c>
       <c r="K26" s="3">
-        <f t="shared" si="5"/>
-        <v>60</v>
+        <f>SUM(E26:J26)</f>
+        <v>40</v>
       </c>
       <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
+      <c r="M26" s="3">
+        <v>50</v>
+      </c>
       <c r="N26" s="3">
         <f>K26-L26-M26</f>
-        <v>60</v>
+        <v>-10</v>
       </c>
       <c r="O26" s="11" t="s">
         <v>97</v>
@@ -2345,35 +2348,37 @@
         <v>8</v>
       </c>
       <c r="E27" s="3">
-        <f t="shared" si="4"/>
+        <f>E$2*$D27</f>
         <v>80</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" si="6"/>
+        <f>F$2*$D27</f>
         <v>80</v>
       </c>
       <c r="G27" s="3">
-        <f t="shared" si="6"/>
+        <f>G$2*$D27</f>
         <v>48</v>
       </c>
       <c r="H27" s="3">
-        <f t="shared" si="6"/>
+        <f>H$2*$D27</f>
         <v>16</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3">
-        <f t="shared" si="7"/>
+        <f>J$2*$D27</f>
         <v>16</v>
       </c>
       <c r="K27" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(E27:J27)</f>
         <v>240</v>
       </c>
       <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
+      <c r="M27" s="3">
+        <v>250</v>
+      </c>
       <c r="N27" s="3">
-        <f t="shared" si="1"/>
-        <v>240</v>
+        <f>K27-L27-M27</f>
+        <v>-10</v>
       </c>
       <c r="O27" s="11" t="s">
         <v>94</v>
@@ -2406,38 +2411,40 @@
         <v>4</v>
       </c>
       <c r="E28" s="3">
-        <f t="shared" si="4"/>
+        <f>E$2*$D28</f>
         <v>40</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" si="6"/>
+        <f>F$2*$D28</f>
         <v>40</v>
       </c>
       <c r="G28" s="3">
-        <f t="shared" si="6"/>
+        <f>G$2*$D28</f>
         <v>24</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" si="6"/>
+        <f>H$2*$D28</f>
         <v>8</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="3">
-        <f t="shared" si="7"/>
+        <f>J$2*$D28</f>
         <v>8</v>
       </c>
       <c r="K28" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(E28:J28)</f>
         <v>120</v>
       </c>
       <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
+      <c r="M28" s="3">
+        <v>150</v>
+      </c>
       <c r="N28" s="3">
         <f>K28-L28-M28</f>
-        <v>120</v>
+        <v>-30</v>
       </c>
       <c r="O28" s="11" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
@@ -2481,14 +2488,16 @@
         <v>2</v>
       </c>
       <c r="K29" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(E29:J29)</f>
         <v>10</v>
       </c>
       <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
+      <c r="M29" s="3">
+        <v>10</v>
+      </c>
       <c r="N29" s="3">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f>K29-L29-M29</f>
+        <v>0</v>
       </c>
       <c r="O29" s="11" t="s">
         <v>90</v>
@@ -2591,19 +2600,19 @@
         <v>1</v>
       </c>
       <c r="E32" s="3">
-        <f t="shared" ref="E32:H33" si="8">E$2*$D32</f>
+        <f>E$2*$D32</f>
         <v>10</v>
       </c>
       <c r="F32" s="3">
-        <f t="shared" si="8"/>
+        <f>F$2*$D32</f>
         <v>10</v>
       </c>
       <c r="G32" s="3">
-        <f t="shared" si="8"/>
+        <f>G$2*$D32</f>
         <v>6</v>
       </c>
       <c r="H32" s="3">
-        <f t="shared" si="8"/>
+        <f>H$2*$D32</f>
         <v>2</v>
       </c>
       <c r="I32" s="3">
@@ -2614,14 +2623,16 @@
         <v>2</v>
       </c>
       <c r="K32" s="3">
-        <f t="shared" ref="K32:K41" si="9">SUM(E32:J32)</f>
+        <f>SUM(E32:J32)</f>
         <v>34</v>
       </c>
-      <c r="L32" s="3"/>
+      <c r="L32" s="3">
+        <v>34</v>
+      </c>
       <c r="M32" s="3"/>
       <c r="N32" s="3">
-        <f t="shared" si="1"/>
-        <v>34</v>
+        <f>K32-L32-M32</f>
+        <v>0</v>
       </c>
       <c r="O32" s="11" t="s">
         <v>75</v>
@@ -2654,19 +2665,19 @@
         <v>1</v>
       </c>
       <c r="E33" s="3">
-        <f t="shared" si="8"/>
+        <f>E$2*$D33</f>
         <v>10</v>
       </c>
       <c r="F33" s="3">
-        <f t="shared" si="8"/>
+        <f>F$2*$D33</f>
         <v>10</v>
       </c>
       <c r="G33" s="3">
-        <f t="shared" si="8"/>
+        <f>G$2*$D33</f>
         <v>6</v>
       </c>
       <c r="H33" s="3">
-        <f t="shared" si="8"/>
+        <f>H$2*$D33</f>
         <v>2</v>
       </c>
       <c r="I33" s="3">
@@ -2677,14 +2688,16 @@
         <v>2</v>
       </c>
       <c r="K33" s="3">
-        <f t="shared" si="9"/>
+        <f>SUM(E33:J33)</f>
         <v>34</v>
       </c>
-      <c r="L33" s="3"/>
+      <c r="L33" s="3">
+        <v>40</v>
+      </c>
       <c r="M33" s="3"/>
       <c r="N33" s="3">
-        <f t="shared" si="1"/>
-        <v>34</v>
+        <f>K33-L33-M33</f>
+        <v>-6</v>
       </c>
       <c r="O33" s="11" t="s">
         <v>75</v>
@@ -2735,14 +2748,18 @@
         <v>2</v>
       </c>
       <c r="K34" s="3">
-        <f t="shared" si="9"/>
+        <f>SUM(E34:J34)</f>
         <v>30</v>
       </c>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
+      <c r="L34" s="3">
+        <v>18</v>
+      </c>
+      <c r="M34" s="3">
+        <v>12</v>
+      </c>
       <c r="N34" s="3">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <f>K34-L34-M34</f>
+        <v>0</v>
       </c>
       <c r="O34" s="11" t="s">
         <v>75</v>
@@ -2789,7 +2806,7 @@
         <v>2</v>
       </c>
       <c r="K35" s="3">
-        <f t="shared" si="9"/>
+        <f>SUM(E35:J35)</f>
         <v>12</v>
       </c>
       <c r="L35" s="3">
@@ -2797,7 +2814,7 @@
       </c>
       <c r="M35" s="3"/>
       <c r="N35" s="3">
-        <f t="shared" si="1"/>
+        <f>K35-L35-M35</f>
         <v>-1</v>
       </c>
       <c r="O35" s="11" t="s">
@@ -2845,14 +2862,16 @@
         <v>2</v>
       </c>
       <c r="K36" s="3">
-        <f t="shared" si="9"/>
+        <f>SUM(E36:J36)</f>
         <v>12</v>
       </c>
       <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
+      <c r="M36" s="3">
+        <v>15</v>
+      </c>
       <c r="N36" s="3">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f>K36-L36-M36</f>
+        <v>-3</v>
       </c>
       <c r="O36" s="11" t="s">
         <v>52</v>
@@ -2899,7 +2918,7 @@
         <v>2</v>
       </c>
       <c r="K37" s="3">
-        <f t="shared" si="9"/>
+        <f>SUM(E37:J37)</f>
         <v>12</v>
       </c>
       <c r="L37" s="3">
@@ -2907,7 +2926,7 @@
       </c>
       <c r="M37" s="3"/>
       <c r="N37" s="3">
-        <f t="shared" si="1"/>
+        <f>K37-L37-M37</f>
         <v>-6</v>
       </c>
       <c r="O37" s="11" t="s">
@@ -2955,13 +2974,13 @@
         <v>0</v>
       </c>
       <c r="K38" s="3">
-        <f t="shared" si="9"/>
+        <f>SUM(E38:J38)</f>
         <v>6</v>
       </c>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3">
-        <f t="shared" si="1"/>
+        <f>K38-L38-M38</f>
         <v>6</v>
       </c>
       <c r="O38" s="11" t="s">
@@ -3011,16 +3030,16 @@
         <v>1</v>
       </c>
       <c r="K39" s="3">
-        <f t="shared" si="9"/>
+        <f>SUM(E39:J39)</f>
         <v>8</v>
       </c>
       <c r="L39" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M39" s="3"/>
       <c r="N39" s="3">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <f>K39-L39-M39</f>
+        <v>0</v>
       </c>
       <c r="O39" s="11" t="s">
         <v>75</v>
@@ -3069,7 +3088,7 @@
         <v>3</v>
       </c>
       <c r="K40" s="3">
-        <f t="shared" si="9"/>
+        <f>SUM(E40:J40)</f>
         <v>24</v>
       </c>
       <c r="L40" s="3">
@@ -3077,7 +3096,7 @@
       </c>
       <c r="M40" s="3"/>
       <c r="N40" s="3">
-        <f t="shared" si="1"/>
+        <f>K40-L40-M40</f>
         <v>-4</v>
       </c>
       <c r="O40" s="12" t="s">
@@ -3127,16 +3146,16 @@
         <v>3</v>
       </c>
       <c r="K41" s="3">
-        <f t="shared" si="9"/>
+        <f>SUM(E41:J41)</f>
         <v>24</v>
       </c>
       <c r="L41" s="3">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="M41" s="3"/>
       <c r="N41" s="3">
-        <f t="shared" si="1"/>
-        <v>21</v>
+        <f>K41-L41-M41</f>
+        <v>0</v>
       </c>
       <c r="O41" s="11" t="s">
         <v>75</v>
@@ -3218,14 +3237,16 @@
         <v>2</v>
       </c>
       <c r="K43" s="3">
-        <f t="shared" ref="K43:K55" si="10">SUM(E43:J43)</f>
+        <f>SUM(E43:J43)</f>
         <v>30</v>
       </c>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
+      <c r="L43" s="3">
+        <v>10</v>
+      </c>
+      <c r="M43" s="1"/>
       <c r="N43" s="3">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <f>K43-M43-L43</f>
+        <v>20</v>
       </c>
       <c r="O43" s="11" t="s">
         <v>78</v>
@@ -3278,14 +3299,16 @@
         <v>2</v>
       </c>
       <c r="K44" s="3">
-        <f t="shared" si="10"/>
+        <f>SUM(E44:J44)</f>
         <v>16</v>
       </c>
       <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
+      <c r="M44" s="3">
+        <v>16</v>
+      </c>
       <c r="N44" s="3">
         <f>K44-L44-M44</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="O44" s="11" t="s">
         <v>75</v>
@@ -3321,15 +3344,15 @@
         <v>0</v>
       </c>
       <c r="F45" s="3">
-        <f t="shared" ref="F45:H55" si="11">F$2*$D45</f>
+        <f>F$2*$D45</f>
         <v>50</v>
       </c>
       <c r="G45" s="3">
-        <f t="shared" si="11"/>
+        <f>G$2*$D45</f>
         <v>30</v>
       </c>
       <c r="H45" s="3">
-        <f t="shared" si="11"/>
+        <f>H$2*$D45</f>
         <v>10</v>
       </c>
       <c r="I45" s="3"/>
@@ -3337,13 +3360,13 @@
         <v>20</v>
       </c>
       <c r="K45" s="3">
-        <f t="shared" si="10"/>
+        <f>SUM(E45:J45)</f>
         <v>110</v>
       </c>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
       <c r="N45" s="3">
-        <f t="shared" si="1"/>
+        <f>K45-L45-M45</f>
         <v>110</v>
       </c>
       <c r="O45" s="11" t="s">
@@ -3377,28 +3400,28 @@
         <v>5</v>
       </c>
       <c r="E46" s="3">
-        <f t="shared" ref="E46:E55" si="12">E$2*$D46</f>
+        <f>E$2*$D46</f>
         <v>50</v>
       </c>
       <c r="F46" s="3">
-        <f t="shared" si="11"/>
+        <f>F$2*$D46</f>
         <v>50</v>
       </c>
       <c r="G46" s="3">
-        <f t="shared" si="11"/>
+        <f>G$2*$D46</f>
         <v>30</v>
       </c>
       <c r="H46" s="3">
-        <f t="shared" si="11"/>
+        <f>H$2*$D46</f>
         <v>10</v>
       </c>
       <c r="I46" s="3"/>
       <c r="J46" s="3">
-        <f t="shared" ref="J46:J55" si="13">J$2*$D46</f>
+        <f>J$2*$D46</f>
         <v>10</v>
       </c>
       <c r="K46" s="3">
-        <f t="shared" si="10"/>
+        <f>SUM(E46:J46)</f>
         <v>150</v>
       </c>
       <c r="L46" s="3">
@@ -3406,7 +3429,7 @@
       </c>
       <c r="M46" s="3"/>
       <c r="N46" s="3">
-        <f t="shared" si="1"/>
+        <f>K46-L46-M46</f>
         <v>50</v>
       </c>
       <c r="O46" s="11" t="s">
@@ -3438,34 +3461,34 @@
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3">
-        <f t="shared" si="12"/>
+        <f>E$2*$D47</f>
         <v>0</v>
       </c>
       <c r="F47" s="3">
-        <f t="shared" si="11"/>
+        <f>F$2*$D47</f>
         <v>0</v>
       </c>
       <c r="G47" s="3">
-        <f t="shared" si="11"/>
+        <f>G$2*$D47</f>
         <v>0</v>
       </c>
       <c r="H47" s="3">
-        <f t="shared" si="11"/>
+        <f>H$2*$D47</f>
         <v>0</v>
       </c>
       <c r="I47" s="3"/>
       <c r="J47" s="3">
-        <f t="shared" si="13"/>
+        <f>J$2*$D47</f>
         <v>0</v>
       </c>
       <c r="K47" s="3">
-        <f t="shared" si="10"/>
+        <f>SUM(E47:J47)</f>
         <v>0</v>
       </c>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
       <c r="N47" s="3">
-        <f t="shared" si="1"/>
+        <f>K47-L47-M47</f>
         <v>0</v>
       </c>
       <c r="O47" s="14"/>
@@ -3522,10 +3545,12 @@
         <v>30</v>
       </c>
       <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
+      <c r="M48" s="3">
+        <v>50</v>
+      </c>
       <c r="N48" s="3">
         <f>K48-L48-M48</f>
-        <v>30</v>
+        <v>-20</v>
       </c>
       <c r="O48" s="11" t="s">
         <v>111</v>
@@ -3583,10 +3608,12 @@
         <v>30</v>
       </c>
       <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
+      <c r="M49" s="3">
+        <v>50</v>
+      </c>
       <c r="N49" s="3">
         <f>K49-L49-M49</f>
-        <v>30</v>
+        <v>-20</v>
       </c>
       <c r="O49" s="11" t="s">
         <v>110</v>
@@ -3618,35 +3645,37 @@
         <v>2</v>
       </c>
       <c r="E50" s="3">
-        <f t="shared" ref="E50:H52" si="14">E$2*$D50</f>
+        <f>E$2*$D50</f>
         <v>20</v>
       </c>
       <c r="F50" s="3">
-        <f t="shared" si="14"/>
+        <f>F$2*$D50</f>
         <v>20</v>
       </c>
       <c r="G50" s="3">
-        <f t="shared" si="14"/>
+        <f>G$2*$D50</f>
         <v>12</v>
       </c>
       <c r="H50" s="3">
-        <f t="shared" si="14"/>
+        <f>H$2*$D50</f>
         <v>4</v>
       </c>
       <c r="I50" s="3"/>
       <c r="J50" s="3">
-        <f t="shared" ref="J50:J52" si="15">J$2*$D50</f>
+        <f>J$2*$D50</f>
         <v>4</v>
       </c>
       <c r="K50" s="3">
-        <f t="shared" ref="K50:K52" si="16">SUM(E50:J50)</f>
+        <f>SUM(E50:J50)</f>
         <v>60</v>
       </c>
       <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
+      <c r="M50" s="3">
+        <v>100</v>
+      </c>
       <c r="N50" s="3">
-        <f t="shared" ref="N50:N52" si="17">K50-L50-M50</f>
-        <v>60</v>
+        <f>K50-L50-M50</f>
+        <v>-40</v>
       </c>
       <c r="O50" s="11" t="s">
         <v>112</v>
@@ -3664,35 +3693,37 @@
         <v>1</v>
       </c>
       <c r="E51" s="3">
-        <f t="shared" si="14"/>
+        <f>E$2*$D51</f>
         <v>10</v>
       </c>
       <c r="F51" s="3">
-        <f t="shared" si="14"/>
+        <f>F$2*$D51</f>
         <v>10</v>
       </c>
       <c r="G51" s="3">
-        <f t="shared" si="14"/>
+        <f>G$2*$D51</f>
         <v>6</v>
       </c>
       <c r="H51" s="3">
-        <f t="shared" si="14"/>
+        <f>H$2*$D51</f>
         <v>2</v>
       </c>
       <c r="I51" s="3"/>
       <c r="J51" s="3">
-        <f t="shared" si="15"/>
+        <f>J$2*$D51</f>
         <v>2</v>
       </c>
       <c r="K51" s="3">
-        <f t="shared" si="16"/>
+        <f>SUM(E51:J51)</f>
         <v>30</v>
       </c>
       <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
+      <c r="M51" s="3">
+        <v>50</v>
+      </c>
       <c r="N51" s="3">
-        <f t="shared" si="17"/>
-        <v>30</v>
+        <f>K51-L51-M51</f>
+        <v>-20</v>
       </c>
       <c r="O51" s="11" t="s">
         <v>113</v>
@@ -3725,35 +3756,37 @@
         <v>1</v>
       </c>
       <c r="E52" s="3">
-        <f t="shared" si="14"/>
+        <f>E$2*$D52</f>
         <v>10</v>
       </c>
       <c r="F52" s="3">
-        <f t="shared" si="14"/>
+        <f>F$2*$D52</f>
         <v>10</v>
       </c>
       <c r="G52" s="3">
-        <f t="shared" si="14"/>
+        <f>G$2*$D52</f>
         <v>6</v>
       </c>
       <c r="H52" s="3">
-        <f t="shared" si="14"/>
+        <f>H$2*$D52</f>
         <v>2</v>
       </c>
       <c r="I52" s="3"/>
       <c r="J52" s="3">
-        <f t="shared" si="15"/>
+        <f>J$2*$D52</f>
         <v>2</v>
       </c>
       <c r="K52" s="3">
-        <f t="shared" si="16"/>
+        <f>SUM(E52:J52)</f>
         <v>30</v>
       </c>
       <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
+      <c r="M52" s="3">
+        <v>50</v>
+      </c>
       <c r="N52" s="3">
-        <f t="shared" si="17"/>
-        <v>30</v>
+        <f>K52-L52-M52</f>
+        <v>-20</v>
       </c>
       <c r="O52" s="11" t="s">
         <v>114</v>
@@ -3820,37 +3853,39 @@
         <v>1</v>
       </c>
       <c r="E54" s="3">
-        <f t="shared" si="12"/>
+        <f>E$2*$D54</f>
         <v>10</v>
       </c>
       <c r="F54" s="3">
-        <f t="shared" si="11"/>
+        <f>F$2*$D54</f>
         <v>10</v>
       </c>
       <c r="G54" s="3">
-        <f t="shared" si="11"/>
+        <f>G$2*$D54</f>
         <v>6</v>
       </c>
       <c r="H54" s="3">
-        <f t="shared" si="11"/>
+        <f>H$2*$D54</f>
         <v>2</v>
       </c>
       <c r="I54" s="3"/>
       <c r="J54" s="3">
-        <f t="shared" si="13"/>
+        <f>J$2*$D54</f>
         <v>2</v>
       </c>
       <c r="K54" s="3">
-        <f t="shared" si="10"/>
+        <f>SUM(E54:J54)</f>
         <v>30</v>
       </c>
       <c r="L54" s="3">
         <v>10</v>
       </c>
-      <c r="M54" s="3"/>
+      <c r="M54" s="3">
+        <v>25</v>
+      </c>
       <c r="N54" s="3">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <f>K54-L54-M54</f>
+        <v>-5</v>
       </c>
       <c r="O54" s="12" t="s">
         <v>59</v>
@@ -3883,28 +3918,28 @@
         <v>1</v>
       </c>
       <c r="E55" s="3">
-        <f t="shared" si="12"/>
+        <f>E$2*$D55</f>
         <v>10</v>
       </c>
       <c r="F55" s="3">
-        <f t="shared" si="11"/>
+        <f>F$2*$D55</f>
         <v>10</v>
       </c>
       <c r="G55" s="3">
-        <f t="shared" si="11"/>
+        <f>G$2*$D55</f>
         <v>6</v>
       </c>
       <c r="H55" s="3">
-        <f t="shared" si="11"/>
+        <f>H$2*$D55</f>
         <v>2</v>
       </c>
       <c r="I55" s="3"/>
       <c r="J55" s="3">
-        <f t="shared" si="13"/>
+        <f>J$2*$D55</f>
         <v>2</v>
       </c>
       <c r="K55" s="3">
-        <f t="shared" si="10"/>
+        <f>SUM(E55:J55)</f>
         <v>30</v>
       </c>
       <c r="L55" s="3">
@@ -3912,7 +3947,7 @@
       </c>
       <c r="M55" s="3"/>
       <c r="N55" s="3">
-        <f t="shared" si="1"/>
+        <f>K55-L55-M55</f>
         <v>0</v>
       </c>
       <c r="O55" s="12" t="s">
@@ -3980,19 +4015,19 @@
         <v>1</v>
       </c>
       <c r="E57" s="3">
-        <f t="shared" ref="E57:H61" si="18">E$2*$D57</f>
+        <f>E$2*$D57</f>
         <v>10</v>
       </c>
       <c r="F57" s="3">
-        <f t="shared" si="18"/>
+        <f>F$2*$D57</f>
         <v>10</v>
       </c>
       <c r="G57" s="3">
-        <f t="shared" si="18"/>
+        <f>G$2*$D57</f>
         <v>6</v>
       </c>
       <c r="H57" s="3">
-        <f t="shared" si="18"/>
+        <f>H$2*$D57</f>
         <v>2</v>
       </c>
       <c r="I57" s="3"/>
@@ -4001,14 +4036,16 @@
         <v>2</v>
       </c>
       <c r="K57" s="3">
-        <f t="shared" ref="K57:K66" si="19">SUM(E57:J57)</f>
+        <f>SUM(E57:J57)</f>
         <v>30</v>
       </c>
-      <c r="L57" s="3"/>
-      <c r="M57" s="3"/>
+      <c r="L57" s="3">
+        <v>30</v>
+      </c>
+      <c r="M57" s="1"/>
       <c r="N57" s="3">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <f>K57-M57-L57</f>
+        <v>0</v>
       </c>
       <c r="O57" s="11" t="s">
         <v>78</v>
@@ -4041,19 +4078,19 @@
         <v>1</v>
       </c>
       <c r="E58" s="3">
-        <f t="shared" si="18"/>
+        <f>E$2*$D58</f>
         <v>10</v>
       </c>
       <c r="F58" s="3">
-        <f t="shared" si="18"/>
+        <f>F$2*$D58</f>
         <v>10</v>
       </c>
       <c r="G58" s="3">
-        <f t="shared" si="18"/>
+        <f>G$2*$D58</f>
         <v>6</v>
       </c>
       <c r="H58" s="3">
-        <f t="shared" si="18"/>
+        <f>H$2*$D58</f>
         <v>2</v>
       </c>
       <c r="I58" s="3"/>
@@ -4062,16 +4099,18 @@
         <v>2</v>
       </c>
       <c r="K58" s="3">
-        <f t="shared" si="19"/>
+        <f>SUM(E58:J58)</f>
         <v>30</v>
       </c>
       <c r="L58" s="3">
         <v>10</v>
       </c>
-      <c r="M58" s="3"/>
+      <c r="M58" s="3">
+        <v>25</v>
+      </c>
       <c r="N58" s="3">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <f>K58-L58-M58</f>
+        <v>-5</v>
       </c>
       <c r="O58" s="11" t="s">
         <v>82</v>
@@ -4104,19 +4143,19 @@
         <v>1</v>
       </c>
       <c r="E59" s="3">
-        <f t="shared" si="18"/>
+        <f>E$2*$D59</f>
         <v>10</v>
       </c>
       <c r="F59" s="3">
-        <f t="shared" si="18"/>
+        <f>F$2*$D59</f>
         <v>10</v>
       </c>
       <c r="G59" s="3">
-        <f t="shared" si="18"/>
+        <f>G$2*$D59</f>
         <v>6</v>
       </c>
       <c r="H59" s="3">
-        <f t="shared" si="18"/>
+        <f>H$2*$D59</f>
         <v>2</v>
       </c>
       <c r="I59" s="3"/>
@@ -4125,16 +4164,18 @@
         <v>2</v>
       </c>
       <c r="K59" s="3">
-        <f t="shared" si="19"/>
+        <f>SUM(E59:J59)</f>
         <v>30</v>
       </c>
       <c r="L59" s="3">
         <v>10</v>
       </c>
-      <c r="M59" s="3"/>
+      <c r="M59" s="3">
+        <v>25</v>
+      </c>
       <c r="N59" s="3">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <f>K59-L59-M59</f>
+        <v>-5</v>
       </c>
       <c r="O59" s="11" t="s">
         <v>81</v>
@@ -4167,19 +4208,19 @@
         <v>6</v>
       </c>
       <c r="E60" s="3">
-        <f t="shared" si="18"/>
+        <f>E$2*$D60</f>
         <v>60</v>
       </c>
       <c r="F60" s="3">
-        <f t="shared" si="18"/>
+        <f>F$2*$D60</f>
         <v>60</v>
       </c>
       <c r="G60" s="3">
-        <f t="shared" si="18"/>
+        <f>G$2*$D60</f>
         <v>36</v>
       </c>
       <c r="H60" s="3">
-        <f t="shared" si="18"/>
+        <f>H$2*$D60</f>
         <v>12</v>
       </c>
       <c r="I60" s="3"/>
@@ -4188,14 +4229,16 @@
         <v>12</v>
       </c>
       <c r="K60" s="3">
-        <f t="shared" si="19"/>
+        <f>SUM(E60:J60)</f>
         <v>180</v>
       </c>
       <c r="L60" s="3"/>
-      <c r="M60" s="3"/>
+      <c r="M60" s="3">
+        <v>200</v>
+      </c>
       <c r="N60" s="3">
-        <f t="shared" si="1"/>
-        <v>180</v>
+        <f>K60-L60-M60</f>
+        <v>-20</v>
       </c>
       <c r="O60" s="11" t="s">
         <v>84</v>
@@ -4228,19 +4271,19 @@
         <v>1</v>
       </c>
       <c r="E61" s="3">
-        <f t="shared" si="18"/>
+        <f>E$2*$D61</f>
         <v>10</v>
       </c>
       <c r="F61" s="3">
-        <f t="shared" si="18"/>
+        <f>F$2*$D61</f>
         <v>10</v>
       </c>
       <c r="G61" s="3">
-        <f t="shared" si="18"/>
+        <f>G$2*$D61</f>
         <v>6</v>
       </c>
       <c r="H61" s="3">
-        <f t="shared" si="18"/>
+        <f>H$2*$D61</f>
         <v>2</v>
       </c>
       <c r="I61" s="3"/>
@@ -4249,14 +4292,16 @@
         <v>2</v>
       </c>
       <c r="K61" s="3">
-        <f t="shared" si="19"/>
+        <f>SUM(E61:J61)</f>
         <v>30</v>
       </c>
       <c r="L61" s="3"/>
-      <c r="M61" s="3"/>
+      <c r="M61" s="3">
+        <v>50</v>
+      </c>
       <c r="N61" s="3">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <f>K61-L61-M61</f>
+        <v>-20</v>
       </c>
       <c r="O61" s="11" t="s">
         <v>83</v>
@@ -4323,19 +4368,19 @@
         <v>1</v>
       </c>
       <c r="E63" s="3">
-        <f t="shared" ref="E63:H66" si="20">E$2*$D63</f>
+        <f>E$2*$D63</f>
         <v>10</v>
       </c>
       <c r="F63" s="3">
-        <f t="shared" si="20"/>
+        <f>F$2*$D63</f>
         <v>10</v>
       </c>
       <c r="G63" s="3">
-        <f t="shared" si="20"/>
+        <f>G$2*$D63</f>
         <v>6</v>
       </c>
       <c r="H63" s="3">
-        <f t="shared" si="20"/>
+        <f>H$2*$D63</f>
         <v>2</v>
       </c>
       <c r="I63" s="3"/>
@@ -4344,14 +4389,16 @@
         <v>2</v>
       </c>
       <c r="K63" s="3">
-        <f t="shared" si="19"/>
+        <f>SUM(E63:J63)</f>
         <v>30</v>
       </c>
-      <c r="L63" s="3"/>
-      <c r="M63" s="3"/>
+      <c r="L63" s="3">
+        <v>30</v>
+      </c>
+      <c r="M63" s="1"/>
       <c r="N63" s="3">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <f>K63-M63-L63</f>
+        <v>0</v>
       </c>
       <c r="O63" s="11" t="s">
         <v>78</v>
@@ -4384,19 +4431,19 @@
         <v>1</v>
       </c>
       <c r="E64" s="3">
-        <f t="shared" si="20"/>
+        <f>E$2*$D64</f>
         <v>10</v>
       </c>
       <c r="F64" s="3">
-        <f t="shared" si="20"/>
+        <f>F$2*$D64</f>
         <v>10</v>
       </c>
       <c r="G64" s="3">
-        <f t="shared" si="20"/>
+        <f>G$2*$D64</f>
         <v>6</v>
       </c>
       <c r="H64" s="3">
-        <f t="shared" si="20"/>
+        <f>H$2*$D64</f>
         <v>2</v>
       </c>
       <c r="I64" s="3"/>
@@ -4408,11 +4455,13 @@
         <f>SUM(E64:J64)</f>
         <v>30</v>
       </c>
-      <c r="L64" s="3"/>
+      <c r="L64" s="3">
+        <v>30</v>
+      </c>
       <c r="M64" s="3"/>
       <c r="N64" s="3">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <f>K64-L64-M64</f>
+        <v>0</v>
       </c>
       <c r="O64" s="11" t="s">
         <v>78</v>
@@ -4445,19 +4494,19 @@
         <v>1</v>
       </c>
       <c r="E65" s="3">
-        <f t="shared" si="20"/>
+        <f>E$2*$D65</f>
         <v>10</v>
       </c>
       <c r="F65" s="3">
-        <f t="shared" si="20"/>
+        <f>F$2*$D65</f>
         <v>10</v>
       </c>
       <c r="G65" s="3">
-        <f t="shared" si="20"/>
+        <f>G$2*$D65</f>
         <v>6</v>
       </c>
       <c r="H65" s="3">
-        <f t="shared" si="20"/>
+        <f>H$2*$D65</f>
         <v>2</v>
       </c>
       <c r="I65" s="3"/>
@@ -4466,14 +4515,16 @@
         <v>2</v>
       </c>
       <c r="K65" s="3">
-        <f t="shared" si="19"/>
+        <f>SUM(E65:J65)</f>
         <v>30</v>
       </c>
       <c r="L65" s="3"/>
-      <c r="M65" s="3"/>
+      <c r="M65" s="3">
+        <v>50</v>
+      </c>
       <c r="N65" s="3">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <f>K65-L65-M65</f>
+        <v>-20</v>
       </c>
       <c r="O65" s="11" t="s">
         <v>105</v>
@@ -4505,19 +4556,19 @@
         <v>1</v>
       </c>
       <c r="E66" s="3">
-        <f t="shared" si="20"/>
+        <f>E$2*$D66</f>
         <v>10</v>
       </c>
       <c r="F66" s="3">
-        <f t="shared" si="20"/>
+        <f>F$2*$D66</f>
         <v>10</v>
       </c>
       <c r="G66" s="3">
-        <f t="shared" si="20"/>
+        <f>G$2*$D66</f>
         <v>6</v>
       </c>
       <c r="H66" s="3">
-        <f t="shared" si="20"/>
+        <f>H$2*$D66</f>
         <v>2</v>
       </c>
       <c r="I66" s="3"/>
@@ -4526,14 +4577,16 @@
         <v>2</v>
       </c>
       <c r="K66" s="3">
-        <f t="shared" si="19"/>
+        <f>SUM(E66:J66)</f>
         <v>30</v>
       </c>
       <c r="L66" s="3"/>
-      <c r="M66" s="3"/>
+      <c r="M66" s="3">
+        <v>100</v>
+      </c>
       <c r="N66" s="3">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <f>K66-L66-M66</f>
+        <v>-70</v>
       </c>
       <c r="O66" s="11" t="s">
         <v>106</v>
@@ -4619,11 +4672,13 @@
         <f>SUM(E68:J68)</f>
         <v>24</v>
       </c>
-      <c r="L68" s="3"/>
+      <c r="L68" s="3">
+        <v>25</v>
+      </c>
       <c r="M68" s="3"/>
       <c r="N68" s="3">
-        <f t="shared" si="1"/>
-        <v>24</v>
+        <f>K68-L68-M68</f>
+        <v>-1</v>
       </c>
       <c r="O68" s="11" t="s">
         <v>101</v>
@@ -4676,10 +4731,12 @@
       <c r="L69" s="3">
         <v>9</v>
       </c>
-      <c r="M69" s="3"/>
+      <c r="M69" s="3">
+        <v>6</v>
+      </c>
       <c r="N69" s="3">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f>K69-L69-M69</f>
+        <v>0</v>
       </c>
       <c r="O69" s="11" t="s">
         <v>102</v>
@@ -4734,7 +4791,7 @@
       <c r="L70" s="3"/>
       <c r="M70" s="3"/>
       <c r="N70" s="3">
-        <f t="shared" si="1"/>
+        <f>K70-L70-M70</f>
         <v>11</v>
       </c>
       <c r="O70" s="11" t="s">
@@ -4757,9 +4814,7 @@
       <c r="AD70" s="2"/>
     </row>
     <row r="71" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A71" s="10">
-        <v>71</v>
-      </c>
+      <c r="A71" s="10"/>
       <c r="B71" s="5"/>
       <c r="C71" s="2"/>
       <c r="D71" s="3"/>
@@ -4791,9 +4846,7 @@
       <c r="AD71" s="2"/>
     </row>
     <row r="72" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A72" s="10">
-        <v>72</v>
-      </c>
+      <c r="A72" s="10"/>
       <c r="B72" s="5"/>
       <c r="C72" s="2"/>
       <c r="D72" s="3"/>
@@ -4825,9 +4878,7 @@
       <c r="AD72" s="2"/>
     </row>
     <row r="73" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A73" s="10">
-        <v>73</v>
-      </c>
+      <c r="A73" s="10"/>
       <c r="B73" s="5"/>
       <c r="C73" s="2"/>
       <c r="D73" s="3"/>
@@ -4859,9 +4910,7 @@
       <c r="AD73" s="2"/>
     </row>
     <row r="74" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A74" s="10">
-        <v>74</v>
-      </c>
+      <c r="A74" s="10"/>
       <c r="B74" s="5"/>
       <c r="C74" s="2"/>
       <c r="D74" s="3"/>
@@ -4893,9 +4942,7 @@
       <c r="AD74" s="2"/>
     </row>
     <row r="75" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A75" s="10">
-        <v>75</v>
-      </c>
+      <c r="A75" s="10"/>
       <c r="B75" s="5"/>
       <c r="C75" s="2"/>
       <c r="D75" s="3"/>
@@ -4927,9 +4974,7 @@
       <c r="AD75" s="2"/>
     </row>
     <row r="76" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A76" s="10">
-        <v>76</v>
-      </c>
+      <c r="A76" s="10"/>
       <c r="B76" s="5"/>
       <c r="C76" s="2"/>
       <c r="D76" s="3"/>
@@ -4961,9 +5006,7 @@
       <c r="AD76" s="2"/>
     </row>
     <row r="77" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A77" s="10">
-        <v>77</v>
-      </c>
+      <c r="A77" s="10"/>
       <c r="B77" s="5"/>
       <c r="C77" s="2"/>
       <c r="D77" s="3"/>
@@ -34848,13 +34891,11 @@
       <c r="AD1040" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="N1:N3 N5:N21 N29:N43 N23:N27 N45:N1048576">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N4">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+  <sortState ref="A1:O1040">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <conditionalFormatting sqref="N29:N43 N24:N27 N45:N1048576 N1:N21">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34863,7 +34904,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N22">
+  <conditionalFormatting sqref="N22:N23">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -34915,16 +34956,22 @@
     <hyperlink ref="O29" r:id="rId39" location="anchorTechnicalDOCS"/>
     <hyperlink ref="O25" r:id="rId40"/>
     <hyperlink ref="O27" r:id="rId41"/>
-    <hyperlink ref="O28" r:id="rId42"/>
-    <hyperlink ref="O45" r:id="rId43"/>
-    <hyperlink ref="O68" r:id="rId44"/>
-    <hyperlink ref="O69" r:id="rId45"/>
-    <hyperlink ref="O70" r:id="rId46"/>
-    <hyperlink ref="O65" r:id="rId47"/>
-    <hyperlink ref="O66" r:id="rId48"/>
+    <hyperlink ref="O45" r:id="rId42"/>
+    <hyperlink ref="O68" r:id="rId43"/>
+    <hyperlink ref="O69" r:id="rId44"/>
+    <hyperlink ref="O70" r:id="rId45"/>
+    <hyperlink ref="O65" r:id="rId46"/>
+    <hyperlink ref="O66" r:id="rId47"/>
+    <hyperlink ref="O26" r:id="rId48"/>
+    <hyperlink ref="O49" r:id="rId49"/>
+    <hyperlink ref="O48" r:id="rId50"/>
+    <hyperlink ref="O50" r:id="rId51"/>
+    <hyperlink ref="O51" r:id="rId52"/>
+    <hyperlink ref="O52" r:id="rId53"/>
+    <hyperlink ref="O28" r:id="rId54"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId49"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId55"/>
 </worksheet>
 </file>
 

</xml_diff>